<commit_message>
voy a subir el proyecto con errores para que lo vea la IA
</commit_message>
<xml_diff>
--- a/data/output/Pedido_Semana_08_09022026_deco_exterior.xlsx
+++ b/data/output/Pedido_Semana_08_09022026_deco_exterior.xlsx
@@ -896,7 +896,7 @@
         <v>2</v>
       </c>
       <c r="Q5" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="3" t="n">
         <v>0</v>
@@ -1434,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="L12" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="4" t="n">
         <v>10.5</v>
@@ -1677,7 +1677,7 @@
         <v>1</v>
       </c>
       <c r="L15" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15" s="4" t="n">
         <v>5.3</v>
@@ -1920,7 +1920,7 @@
         <v>1</v>
       </c>
       <c r="L18" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="4" t="n">
         <v>14.12</v>
@@ -2423,7 +2423,7 @@
         <v>2</v>
       </c>
       <c r="Q24" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R24" s="3" t="n">
         <v>0</v>
@@ -2487,7 +2487,7 @@
         <v>1</v>
       </c>
       <c r="L25" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" s="4" t="n">
         <v>13.48</v>
@@ -2747,7 +2747,7 @@
         <v>3</v>
       </c>
       <c r="Q28" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R28" s="3" t="n">
         <v>0</v>
@@ -2973,7 +2973,7 @@
         <v>1</v>
       </c>
       <c r="L31" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31" s="4" t="n">
         <v>8.699999999999999</v>
@@ -3152,7 +3152,7 @@
         <v>2</v>
       </c>
       <c r="Q33" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R33" s="3" t="n">
         <v>0</v>
@@ -3459,7 +3459,7 @@
         <v>3</v>
       </c>
       <c r="L37" s="3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M37" s="4" t="n">
         <v>4.73</v>
@@ -3557,7 +3557,7 @@
         <v>3</v>
       </c>
       <c r="Q38" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R38" s="3" t="n">
         <v>0</v>
@@ -3864,7 +3864,7 @@
         <v>2</v>
       </c>
       <c r="L42" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M42" s="4" t="n">
         <v>5.1</v>
@@ -4350,7 +4350,7 @@
         <v>1</v>
       </c>
       <c r="L48" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M48" s="4" t="n">
         <v>28.35</v>
@@ -4836,7 +4836,7 @@
         <v>1</v>
       </c>
       <c r="L54" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M54" s="4" t="n">
         <v>18.45</v>
@@ -4934,7 +4934,7 @@
         <v>2</v>
       </c>
       <c r="Q55" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R55" s="3" t="n">
         <v>0</v>
@@ -5015,7 +5015,7 @@
         <v>4</v>
       </c>
       <c r="Q56" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R56" s="3" t="n">
         <v>0</v>
@@ -5258,7 +5258,7 @@
         <v>4</v>
       </c>
       <c r="Q59" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R59" s="3" t="n">
         <v>0</v>
@@ -6230,7 +6230,7 @@
         <v>2</v>
       </c>
       <c r="Q71" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R71" s="3" t="n">
         <v>0</v>
@@ -6392,7 +6392,7 @@
         <v>3</v>
       </c>
       <c r="Q73" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R73" s="3" t="n">
         <v>0</v>
@@ -7023,7 +7023,7 @@
         <v>1</v>
       </c>
       <c r="L81" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M81" s="4" t="n">
         <v>20.67</v>
@@ -7364,7 +7364,7 @@
         <v>3</v>
       </c>
       <c r="Q85" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R85" s="3" t="n">
         <v>0</v>
@@ -7428,7 +7428,7 @@
         <v>3</v>
       </c>
       <c r="L86" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M86" s="4" t="n">
         <v>14.88</v>
@@ -7445,7 +7445,7 @@
         <v>10</v>
       </c>
       <c r="Q86" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R86" s="3" t="n">
         <v>0</v>
@@ -7526,7 +7526,7 @@
         <v>6</v>
       </c>
       <c r="Q87" s="2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R87" s="3" t="n">
         <v>0</v>
@@ -8174,7 +8174,7 @@
         <v>4</v>
       </c>
       <c r="Q95" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R95" s="3" t="n">
         <v>0</v>
@@ -8404,7 +8404,7 @@
         </is>
       </c>
       <c r="C110" s="8" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>